<commit_message>
commit ajuste de inconsistências
</commit_message>
<xml_diff>
--- a/database/anexo b.xlsx
+++ b/database/anexo b.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bb5bd7a50d11ebd7/Área de Trabalho/Programa PYQT6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme\Documents\Licitacao360\pyqt6\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="110" documentId="8_{4F0647EC-2228-4685-9A2A-7A40CD350DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5098D6C-928B-44D0-BF9A-263E3471FF31}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A78153-FBF7-4BBE-A229-0781C6EBA440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="4. Especificação" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="179">
   <si>
     <t>item_num</t>
   </si>
@@ -640,17 +640,2647 @@
   <si>
     <t>Ar-Condicionado 12.000 Btu (Instalação Inclusa) (Cota Reservada ME-EPP)</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/221</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/222</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/223</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/224</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/225</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/226</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/227</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/228</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/229</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/230</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/231</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/232</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/233</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/234</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/235</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/236</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/237</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/238</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/239</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/240</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/241</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/242</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/243</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/244</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/245</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/246</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/247</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/248</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/249</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/250</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/251</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/252</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/253</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/254</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/255</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/256</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/257</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/258</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/259</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/260</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/261</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/262</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/263</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/264</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/265</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/266</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/267</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/268</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/269</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/270</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/271</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/272</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/273</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/274</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/275</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/276</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/277</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/278</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/279</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/280</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Televisor
+Características Adicionais: 4k, 3d E Smart Tv, Mínimo: 2 Usb, 3 Hdmi, Wi-Fi In
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Carlito;Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Tamanho Tela: 75 POL
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tipo Tela: Led
+Voltagem: 110/281</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -681,6 +3311,11 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Carlito;Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -753,22 +3388,22 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -903,10 +3538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AME70"/>
+  <dimension ref="A1:AME131"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69:A131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="15.5"/>
@@ -1899,8 +4534,863 @@
         <v>90</v>
       </c>
     </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="5">
+        <v>70</v>
+      </c>
+      <c r="B71" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="5">
+        <v>71</v>
+      </c>
+      <c r="B72" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D72" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="5">
+        <v>72</v>
+      </c>
+      <c r="B73" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="5">
+        <v>73</v>
+      </c>
+      <c r="B74" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="5">
+        <v>74</v>
+      </c>
+      <c r="B75" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="5">
+        <v>75</v>
+      </c>
+      <c r="B76" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="5">
+        <v>76</v>
+      </c>
+      <c r="B77" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="5">
+        <v>77</v>
+      </c>
+      <c r="B78" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="5">
+        <v>78</v>
+      </c>
+      <c r="B79" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="5">
+        <v>79</v>
+      </c>
+      <c r="B80" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="5">
+        <v>80</v>
+      </c>
+      <c r="B81" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D81" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="5">
+        <v>81</v>
+      </c>
+      <c r="B82" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="5">
+        <v>82</v>
+      </c>
+      <c r="B83" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D83" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="5">
+        <v>83</v>
+      </c>
+      <c r="B84" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D84" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="5">
+        <v>84</v>
+      </c>
+      <c r="B85" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D85" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="5">
+        <v>85</v>
+      </c>
+      <c r="B86" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D86" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="5">
+        <v>86</v>
+      </c>
+      <c r="B87" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="5">
+        <v>87</v>
+      </c>
+      <c r="B88" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D88" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="5">
+        <v>88</v>
+      </c>
+      <c r="B89" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="5">
+        <v>89</v>
+      </c>
+      <c r="B90" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D90" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="5">
+        <v>90</v>
+      </c>
+      <c r="B91" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D91" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="5">
+        <v>91</v>
+      </c>
+      <c r="B92" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D92" s="8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="5">
+        <v>92</v>
+      </c>
+      <c r="B93" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D93" s="8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="5">
+        <v>93</v>
+      </c>
+      <c r="B94" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D94" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="5">
+        <v>94</v>
+      </c>
+      <c r="B95" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D95" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="5">
+        <v>95</v>
+      </c>
+      <c r="B96" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="5">
+        <v>96</v>
+      </c>
+      <c r="B97" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D97" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="5">
+        <v>97</v>
+      </c>
+      <c r="B98" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D98" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="5">
+        <v>98</v>
+      </c>
+      <c r="B99" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D99" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="5">
+        <v>99</v>
+      </c>
+      <c r="B100" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D100" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="5">
+        <v>100</v>
+      </c>
+      <c r="B101" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D101" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="5">
+        <v>101</v>
+      </c>
+      <c r="B102" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D102" s="8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="5">
+        <v>102</v>
+      </c>
+      <c r="B103" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C103" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D103" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="5">
+        <v>103</v>
+      </c>
+      <c r="B104" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D104" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="5">
+        <v>104</v>
+      </c>
+      <c r="B105" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D105" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="5">
+        <v>105</v>
+      </c>
+      <c r="B106" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D106" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="5">
+        <v>106</v>
+      </c>
+      <c r="B107" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C107" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D107" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="5">
+        <v>107</v>
+      </c>
+      <c r="B108" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C108" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D108" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="5">
+        <v>108</v>
+      </c>
+      <c r="B109" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C109" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D109" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" s="5">
+        <v>109</v>
+      </c>
+      <c r="B110" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C110" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D110" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="5">
+        <v>110</v>
+      </c>
+      <c r="B111" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D111" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" s="5">
+        <v>111</v>
+      </c>
+      <c r="B112" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C112" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D112" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" s="5">
+        <v>112</v>
+      </c>
+      <c r="B113" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C113" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D113" s="8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" s="5">
+        <v>113</v>
+      </c>
+      <c r="B114" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C114" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D114" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" s="5">
+        <v>114</v>
+      </c>
+      <c r="B115" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C115" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D115" s="8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" s="5">
+        <v>115</v>
+      </c>
+      <c r="B116" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C116" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D116" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" s="5">
+        <v>116</v>
+      </c>
+      <c r="B117" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C117" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D117" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" s="5">
+        <v>117</v>
+      </c>
+      <c r="B118" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C118" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D118" s="8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" s="5">
+        <v>118</v>
+      </c>
+      <c r="B119" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C119" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D119" s="8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" s="5">
+        <v>119</v>
+      </c>
+      <c r="B120" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C120" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D120" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" s="5">
+        <v>120</v>
+      </c>
+      <c r="B121" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C121" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D121" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" s="5">
+        <v>121</v>
+      </c>
+      <c r="B122" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C122" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D122" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" s="5">
+        <v>122</v>
+      </c>
+      <c r="B123" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C123" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D123" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" s="5">
+        <v>123</v>
+      </c>
+      <c r="B124" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C124" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D124" s="8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" s="5">
+        <v>124</v>
+      </c>
+      <c r="B125" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C125" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D125" s="8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" s="5">
+        <v>125</v>
+      </c>
+      <c r="B126" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C126" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D126" s="8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" s="5">
+        <v>126</v>
+      </c>
+      <c r="B127" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C127" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D127" s="8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" s="5">
+        <v>127</v>
+      </c>
+      <c r="B128" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C128" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D128" s="8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="5">
+        <v>128</v>
+      </c>
+      <c r="B129" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C129" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D129" s="8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="5">
+        <v>129</v>
+      </c>
+      <c r="B130" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C130" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D130" s="8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" s="5">
+        <v>130</v>
+      </c>
+      <c r="B131" s="6">
+        <v>439607</v>
+      </c>
+      <c r="C131" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D131" s="8" t="s">
+        <v>178</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C70" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>